<commit_message>
Copy Files From Source Repo (2025-10-11 14:50)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends 2023.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <r>
       <rPr>
@@ -107,17 +107,6 @@
         <family val="2"/>
       </rPr>
       <t>Pesquisas online para Chai</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>4:36</t>
     </r>
   </si>
   <si>
@@ -872,11 +861,11 @@
       <c r="C6">
         <v>499</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <v>436</v>
+      </c>
+      <c r="E6" t="s">
         <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
       </c>
       <c r="F6">
         <v>2996</v>

</xml_diff>